<commit_message>
Módulo 05 - Formulas: Maiúscula e PRI.maiúscula
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-texto.xlsx
+++ b/módulo 05/aula-formulas-texto.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\05 Primeiras fórmulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBF50C1-A269-46EE-B992-C0B7F813EA36}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{9677FD8D-6660-41E5-9A81-FFEA2AD51EE9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10125" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="8" r:id="rId1"/>
     <sheet name="Cad_Empresa" sheetId="9" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -51,11 +50,26 @@
   <si>
     <t>ENDEREÇO</t>
   </si>
+  <si>
+    <t>transportadora rápida web</t>
+  </si>
+  <si>
+    <t>Pegar o valor tudo maiúsculo: digita o sinal =maiuscula / digita tab/ e clica na céçuça que tem o valor desejado/dá enter</t>
+  </si>
+  <si>
+    <t>Pegar o mesmo conteúdo de texto da célula: clica na célula/insere o sinal = e clica na outra célula/enter</t>
+  </si>
+  <si>
+    <t>Copiar as primeiras letras maiusculas: insere o sinal = juntamente com pri.maiuscula/ tab/clica no conteúdo/enter</t>
+  </si>
+  <si>
+    <t>maria brown silva</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,7 +183,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -252,7 +266,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -372,7 +386,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -453,7 +467,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,7 +545,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -609,7 +623,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,7 +707,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -774,7 +788,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -894,7 +908,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,7 +991,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1055,7 +1069,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1133,7 +1147,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1211,7 +1225,7 @@
         <xdr:cNvPr id="8" name="Retângulo: Cantos Superiores Recortados 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1292,7 +1306,7 @@
         <xdr:cNvPr id="9" name="Retângulo: Cantos Superiores Recortados 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,11 +1670,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46F83BD-F3BF-43E4-9A28-8E259EC6705F}">
-  <dimension ref="A1:P16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1710,29 +1724,56 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="B6" s="5" t="str">
+        <f>Cad_Empresa!B6</f>
+        <v>transportadora rápida web</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="str">
+        <f>UPPER(Cad_Empresa!B6)</f>
+        <v>TRANSPORTADORA RÁPIDA WEB</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H13" s="7"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="str">
+        <f>PROPER(Cad_Empresa!B10)</f>
+        <v>Maria Brown Silva</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1742,11 +1783,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F21D338-352F-44D6-9932-736A440D777F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1796,7 +1837,9 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1807,7 +1850,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1829,7 +1874,9 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
+      <c r="B18" s="6">
+        <v>1234</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">

</xml_diff>

<commit_message>
Módulo 05 - Formulas: Concatenações
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-texto.xlsx
+++ b/módulo 05/aula-formulas-texto.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -64,6 +64,27 @@
   </si>
   <si>
     <t>maria brown silva</t>
+  </si>
+  <si>
+    <t>rua oscar pereira</t>
+  </si>
+  <si>
+    <t>catu</t>
+  </si>
+  <si>
+    <t>Concatenar células(conteúdos) : insere o sinal = juntamente com a fórmula concatenar/ clica na célula /clica no sinal ;</t>
+  </si>
+  <si>
+    <t>seleciona a segunda célula/ quando tiver todas as células que deseja clica no enter</t>
+  </si>
+  <si>
+    <t>Editar fórmula : fn+f2</t>
+  </si>
+  <si>
+    <t>Espaço entre as concatenações: só inserir apas duplas entre os parâmetros isolados pelo sinal ;</t>
+  </si>
+  <si>
+    <t>aninhamento de fórmulas, exemplo: =CONCATENAR(PRI.MAIÚSCULA(Cad_Empresa!B14);</t>
   </si>
 </sst>
 </file>
@@ -130,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -145,6 +166,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,7 +205,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -266,7 +288,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -386,7 +408,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -467,7 +489,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -545,7 +567,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -623,7 +645,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -707,7 +729,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -788,7 +810,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -908,7 +930,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -991,7 +1013,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1069,7 +1091,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1147,7 +1169,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1225,7 +1247,7 @@
         <xdr:cNvPr id="8" name="Retângulo: Cantos Superiores Recortados 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1328,7 @@
         <xdr:cNvPr id="9" name="Retângulo: Cantos Superiores Recortados 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1734,10 +1756,21 @@
         <f>UPPER(Cad_Empresa!B6)</f>
         <v>TRANSPORTADORA RÁPIDA WEB</v>
       </c>
+      <c r="G7" s="8">
+        <v>43520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G8" s="1">
+        <v>0.28299999999999997</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1745,34 +1778,99 @@
         <f>PROPER(Cad_Empresa!B10)</f>
         <v>Maria Brown Silva</v>
       </c>
+      <c r="G10" s="1">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G12" s="7" t="str">
+        <f>TEXT(G10,"R$#.##0,00")</f>
+        <v>R$1.245,00</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G14" s="7" t="str">
+        <f>TEXT(G9,"0000")</f>
+        <v>0234</v>
+      </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G15" s="7" t="str">
+        <f>TEXT(G8,"0,00%")</f>
+        <v>28,30%</v>
+      </c>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="G16" s="7" t="str">
+        <f>TEXT(G7,"dd/mm/aaaa")</f>
+        <v>24/02/2019</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="str">
+        <f>CONCATENATE(PROPER( Cad_Empresa!B14),", Número ",Cad_Empresa!B18," - ", PROPER(Cad_Empresa!B22))</f>
+        <v>Rua Oscar Pereira, Número 1234 - Catu</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f>TEXT(G7,"dd/mm/aa")</f>
+        <v>24/02/19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="7" t="str">
+        <f>TEXT(G7,"dddd")</f>
+        <v>domingo</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="7" t="str">
+        <f>TEXT(G7,"mmmm")</f>
+        <v>fevereiro</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1786,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1863,7 +1961,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1884,7 +1984,9 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>

</xml_diff>